<commit_message>
All Bitbang Created, created generic comm function
</commit_message>
<xml_diff>
--- a/Function Tracker.xlsx
+++ b/Function Tracker.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12720"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="71">
   <si>
     <t>Function</t>
   </si>
@@ -238,6 +238,12 @@
   </si>
   <si>
     <t>Generate the SWD Request</t>
+  </si>
+  <si>
+    <t>uint32_t SWD_Comm(uint8_t command, uint32_t data)</t>
+  </si>
+  <si>
+    <t>Generic function to perform an SWD message</t>
   </si>
 </sst>
 </file>
@@ -557,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +629,7 @@
       </c>
       <c r="J2" s="2">
         <f>SUM(H:H)/(4*(COUNTA(A:A)-1))</f>
-        <v>0.62068965517241381</v>
+        <v>0.68333333333333335</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1033,7 +1039,7 @@
         <v>1</v>
       </c>
       <c r="E18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="1">
         <v>0</v>
@@ -1042,8 +1048,8 @@
         <v>0</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" ref="H18:H32" si="2">SUM(D18:G18)</f>
-        <v>1</v>
+        <f t="shared" ref="H18:H33" si="2">SUM(D18:G18)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1060,7 +1066,7 @@
         <v>1</v>
       </c>
       <c r="E19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="1">
         <v>0</v>
@@ -1070,7 +1076,7 @@
       </c>
       <c r="H19" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -1087,7 +1093,7 @@
         <v>1</v>
       </c>
       <c r="E20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="1">
         <v>0</v>
@@ -1097,7 +1103,7 @@
       </c>
       <c r="H20" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1114,7 +1120,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="1">
         <v>0</v>
@@ -1124,7 +1130,7 @@
       </c>
       <c r="H21" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1141,7 +1147,7 @@
         <v>1</v>
       </c>
       <c r="E22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22" s="1">
         <v>0</v>
@@ -1151,7 +1157,7 @@
       </c>
       <c r="H22" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1210,19 +1216,19 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>44</v>
+        <v>69</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="E25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="1">
         <v>0</v>
@@ -1232,24 +1238,24 @@
       </c>
       <c r="H25" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
       </c>
       <c r="E26" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -1259,24 +1265,24 @@
       </c>
       <c r="H26" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D27" s="1">
         <v>1</v>
       </c>
       <c r="E27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27" s="1">
         <v>0</v>
@@ -1286,18 +1292,18 @@
       </c>
       <c r="H27" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D28" s="1">
         <v>1</v>
@@ -1318,13 +1324,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -1345,13 +1351,13 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D30" s="1">
         <v>1</v>
@@ -1372,13 +1378,13 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
@@ -1399,27 +1405,54 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="1">
-        <v>1</v>
-      </c>
-      <c r="E32" s="1">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1">
-        <v>0</v>
-      </c>
-      <c r="G32" s="1">
-        <v>0</v>
-      </c>
-      <c r="H32" s="1">
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>

</xml_diff>